<commit_message>
danh sach ngay thang
</commit_message>
<xml_diff>
--- a/Data/052018/chamcong.xlsx
+++ b/Data/052018/chamcong.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DucTn\Desktop\Luong\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\html\live\luong.diepxuan.vn\Data\052018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F0C9ABF-34BA-4457-9AFA-D480D2CE856B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C6089EB2-CC18-4574-AE65-3365550478A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,10 +436,10 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32:XFD32"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -527,6 +527,9 @@
       <c r="F2" s="5">
         <v>1</v>
       </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
@@ -644,6 +647,9 @@
       <c r="F7" s="5">
         <v>0</v>
       </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
@@ -824,6 +830,9 @@
       <c r="F14" s="5">
         <v>1</v>
       </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5">
         <v>1</v>
@@ -1294,6 +1303,9 @@
       </c>
       <c r="F28" s="5">
         <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
       </c>
       <c r="H28" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
cap nhat nang suat
</commit_message>
<xml_diff>
--- a/Data/052018/chamcong.xlsx
+++ b/Data/052018/chamcong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\html\live\luong.diepxuan.vn\Data\052018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C6089EB2-CC18-4574-AE65-3365550478A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F211C932-4354-454A-9CE1-FF214ABBC240}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,10 +436,10 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -513,22 +513,22 @@
         <v>43221</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="5"/>
     </row>
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
@@ -645,10 +645,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5">
@@ -894,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <v>1</v>
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G17" s="5">
         <v>1</v>
@@ -999,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="5">
         <v>1</v>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="5">
         <v>1</v>

</xml_diff>